<commit_message>
select option from addNew dropdown
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/demo.xlsx
+++ b/src/test/resources/testdata/demo.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30048" windowHeight="13584" activeTab="1"/>
+    <workbookView windowWidth="26148" windowHeight="13655" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="testERPBook" sheetId="1" r:id="rId1"/>
     <sheet name="testRoad" sheetId="2" r:id="rId2"/>
+    <sheet name="testCyber" sheetId="3" r:id="rId3"/>
+    <sheet name="testPhysic" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Mail</t>
   </si>
@@ -75,6 +77,36 @@
   </si>
   <si>
     <t>https://onlinebusiness.icbc.com/webdeas-ui/login;type=driver</t>
+  </si>
+  <si>
+    <t>CaseID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>PassWord</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>KfNdc&amp;^^f3QA_b4LqdZFvS54d</t>
+  </si>
+  <si>
+    <t>DropDownOption</t>
+  </si>
+  <si>
+    <t>This case is to create a incident report</t>
+  </si>
+  <si>
+    <t>Yk3%2+jUn</t>
+  </si>
+  <si>
+    <t>Incident Report</t>
   </si>
 </sst>
 </file>
@@ -83,9 +115,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -104,8 +136,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -113,6 +146,36 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -126,8 +189,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -143,15 +207,44 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -159,88 +252,27 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -249,13 +281,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -267,169 +443,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,6 +478,65 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -461,8 +558,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -481,217 +578,164 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1070,19 +1114,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -1093,22 +1137,22 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>2369860616</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="6">
         <v>43831.0423726852</v>
       </c>
       <c r="G2">
@@ -1116,22 +1160,22 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>2369860616</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="6">
         <v>43832.0423726852</v>
       </c>
       <c r="G3">
@@ -1139,68 +1183,68 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="4"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1218,8 +1262,8 @@
   <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="4"/>
@@ -1231,16 +1275,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E1" t="s">
@@ -1260,7 +1304,7 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1271,4 +1315,113 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="2" width="10.2222222222222" customWidth="1"/>
+    <col min="3" max="3" width="14.1111111111111" customWidth="1"/>
+    <col min="4" max="4" width="26.4444444444444" customWidth="1"/>
+    <col min="5" max="5" width="16.3333333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="2" width="24.4444444444444" customWidth="1"/>
+    <col min="3" max="4" width="9.88888888888889" customWidth="1"/>
+    <col min="5" max="5" width="15.3333333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add new incident report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/demo.xlsx
+++ b/src/test/resources/testdata/demo.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
   <si>
     <t>Mail</t>
   </si>
@@ -100,6 +100,12 @@
     <t>DropDownOption</t>
   </si>
   <si>
+    <t>ArrestDetails</t>
+  </si>
+  <si>
+    <t>WorkplaceViolence</t>
+  </si>
+  <si>
     <t>This case is to create a incident report</t>
   </si>
   <si>
@@ -107,6 +113,9 @@
   </si>
   <si>
     <t>Incident Report</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -114,10 +123,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -137,30 +146,69 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -174,24 +222,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,60 +253,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -287,25 +296,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -317,157 +374,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,6 +487,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -520,6 +553,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -539,192 +587,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -738,10 +747,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
@@ -1114,19 +1123,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" t="s">
@@ -1275,16 +1284,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E1" t="s">
@@ -1304,7 +1313,7 @@
       <c r="D2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1347,8 +1356,8 @@
       <c r="D1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
@@ -1360,7 +1369,7 @@
       <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1371,20 +1380,21 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
     <col min="2" max="2" width="24.4444444444444" customWidth="1"/>
     <col min="3" max="4" width="9.88888888888889" customWidth="1"/>
-    <col min="5" max="5" width="15.3333333333333" customWidth="1"/>
+    <col min="5" max="6" width="15.3333333333333" customWidth="1"/>
+    <col min="7" max="7" width="16.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -1400,25 +1410,36 @@
       <c r="E1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add comment into excel data
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/demo.xlsx
+++ b/src/test/resources/testdata/demo.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldu\git\d3securityautomation\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC67E79-3C82-41FA-BEED-EE341FECF715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="26148" windowHeight="13655" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="testERPBook" sheetId="1" r:id="rId1"/>
@@ -24,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Mail</t>
   </si>
@@ -113,71 +107,80 @@
     <t>WorkplaceViolence</t>
   </si>
   <si>
+    <t xml:space="preserve">TypeofAccident </t>
+  </si>
+  <si>
+    <t>RequiredField</t>
+  </si>
+  <si>
+    <t>MandatoryonSave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MandatoryonClose </t>
+  </si>
+  <si>
+    <t>//This case is to create a incident report</t>
+  </si>
+  <si>
+    <t>AutomationP2</t>
+  </si>
+  <si>
+    <t>Qa123!</t>
+  </si>
+  <si>
+    <t>Incident Report</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Posture</t>
+  </si>
+  <si>
+    <t>Hitech</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
     <t>This case is to create a incident report</t>
   </si>
   <si>
-    <t>Incident Report</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Posture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TypeofAccident </t>
-  </si>
-  <si>
-    <t>RequiredField</t>
-  </si>
-  <si>
-    <t>Hitech</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MandatoryonClose </t>
-  </si>
-  <si>
-    <t>MandatoryonSave</t>
-  </si>
-  <si>
-    <t>Save</t>
-  </si>
-  <si>
-    <t>Close</t>
+    <t>MandatoryFields</t>
+  </si>
+  <si>
+    <t>OwnerSite</t>
   </si>
   <si>
     <t>This case is to create a case</t>
   </si>
   <si>
+    <t>AutomationP1</t>
+  </si>
+  <si>
     <t>Case Intake</t>
   </si>
   <si>
     <t>YES</t>
   </si>
   <si>
-    <t>OwnerSite</t>
-  </si>
-  <si>
     <t>_Jers Test Site</t>
-  </si>
-  <si>
-    <t>MandatoryFields</t>
-  </si>
-  <si>
-    <t>AutomationP1</t>
-  </si>
-  <si>
-    <t>Qa123!</t>
-  </si>
-  <si>
-    <t>AutomationP2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,10 +193,147 @@
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,8 +346,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -215,12 +541,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -231,28 +796,71 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -539,25 +1147,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="40.140625" customWidth="1"/>
-    <col min="2" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="5" width="23.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="40.1388888888889" customWidth="1"/>
+    <col min="2" max="3" width="8.42592592592593" customWidth="1"/>
+    <col min="4" max="5" width="23.5740740740741" customWidth="1"/>
+    <col min="6" max="6" width="17.8518518518519" customWidth="1"/>
+    <col min="7" max="7" width="11.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -600,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="4">
-        <v>43831.042372685202</v>
+        <v>43831.0423726852</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -623,13 +1231,13 @@
         <v>10</v>
       </c>
       <c r="F3" s="4">
-        <v>43832.042372685202</v>
+        <v>43832.0423726852</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -637,7 +1245,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -645,7 +1253,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:6">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -653,7 +1261,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:6">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -661,7 +1269,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:6">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -669,7 +1277,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:6">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -677,7 +1285,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:6">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -685,7 +1293,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:6">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -695,28 +1303,30 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" tooltip="mailto:goushijie@hotmail.com" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="durongchun@hotmail.com"/>
+    <hyperlink ref="A3" r:id="rId2" display="goushijie@hotmail.com" tooltip="mailto:goushijie@hotmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="A1" sqref="$A1:$XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="58.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.287037037037" customWidth="1"/>
+    <col min="2" max="2" width="20.712962962963" customWidth="1"/>
+    <col min="3" max="3" width="17.8518518518519" customWidth="1"/>
+    <col min="5" max="5" width="58.712962962963" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -755,29 +1365,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://onlinebusiness.icbc.com/webdeas-ui/login;type=driver"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85185185185185" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.287037037037" customWidth="1"/>
+    <col min="3" max="3" width="14.1388888888889" customWidth="1"/>
+    <col min="4" max="4" width="26.4259259259259" customWidth="1"/>
+    <col min="5" max="5" width="16.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -805,26 +1417,28 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85185185185185" defaultRowHeight="14.4" outlineLevelRow="2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="6" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="3" max="4" width="9.85185185185185" customWidth="1"/>
+    <col min="5" max="6" width="15.287037037037" customWidth="1"/>
+    <col min="7" max="7" width="16.287037037037" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.287037037037" customWidth="1"/>
+    <col min="11" max="11" width="19.287037037037" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -850,16 +1464,16 @@
         <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -867,55 +1481,92 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="J2" t="s">
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
         <v>38</v>
       </c>
-      <c r="K2" t="s">
+      <c r="I3" t="s">
         <v>39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAC26E60-850C-4A7E-838F-319A8D5C3F86}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="32.8518518518519" customWidth="1"/>
+    <col min="3" max="3" width="17.4259259259259" customWidth="1"/>
+    <col min="5" max="5" width="17.8518518518519" customWidth="1"/>
+    <col min="6" max="6" width="16.5740740740741" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
   </cols>
   <sheetData>
@@ -936,10 +1587,10 @@
         <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -947,25 +1598,26 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>46</v>
       </c>
       <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
         <v>47</v>
       </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>